<commit_message>
Add calendar view, btnHero on all CTAs, and q10/q11 fuzzy scoring
Calendar tab now has a monthly calendar grid with category-colored dots
and day filtering. All primary CTA buttons use the metallic gradient
btnHero() style. Free-text quiz answers (q10/q11) are now tokenized and
fuzzy-matched against date titles, descriptions, variations, and vibes
to boost relevant scores (+3 for q10, +4 for q11).

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/vela-hooks.xlsx
+++ b/vela-hooks.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vela Hooks &amp; Ad Copy" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Vela Hooks &amp; Ad Copy" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Vela Hooks &amp; Ad Copy'!$A$1:$E$16</definedName>
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -863,6 +863,2506 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Guys, this is for you. Thank me later.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Direct bro-to-bro recommend</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Guys, when it comes to planning date nights with your lady, you can thank me later.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Longer version of the recommend</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>If your girl has to plan her own date night, you already lost.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Guilt + challenge</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Be honest. When's the last time you actually planned a date?</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Direct question — makes them think</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Your girl is tired of 'wanna just get food?' and you know it.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Calls out the lazy default</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>If your date night ideas are dinner and a movie every time, this is for you.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Calls out repetition</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Fellas, 'I don't know, what do you wanna do?' is not a plan.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Mocks the common response</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>She's not asking for a lot. She's asking for effort.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Reframe — effort not money</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>You're not broke. You're just lazy with planning.</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Challenges the excuse</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>If she has to send you a TikTok saying 'we should do this,' you're behind.</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Relatable scenario</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Stop waiting for her to plan everything.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Short and blunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>You have time to scroll for 2 hours but can't plan a date night?</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Time comparison callout</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>If your girl is planning the dates, what exactly are you doing?</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Rhetorical challenge</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>The bar is on the floor and you're still tripping over it.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Funny low-bar callout</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Send this to your boy who hasn't planned a date in 6 months.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Tag/share hook</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>I'm about to save your relationship in 60 seconds.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Bold promise opener</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Bro, I found something that's gonna make you look like a genius.</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Excited discovery tone</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>This is the cheat code for date nights. I'm not gatekeeping.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Cheat code framing</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Fellas, bookmark this. You'll need it this weekend.</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Urgency + save</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>I wish someone showed me this 2 years ago.</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Regret / hindsight</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Every guy needs to know about this app.</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Universal recommendation</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Your girl is about to think you're the most thoughtful person alive.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Outcome promise</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>This is the easiest W you'll ever take in your relationship.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Easy win framing</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>How to go from 'he never plans anything' to 'how did you come up with this?'</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Before/after transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Found something that does all the thinking for you. You're welcome.</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Lazy-friendly sell</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>If you have a girlfriend, you need this.</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Simple direct statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>The secret to never running out of date ideas.</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Secret / curiosity</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>She's gonna ask how you came up with this. Just say you're built different.</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Funny outcome</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>So my girl said 'we never do anything fun' and I took that personally.</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Story opener — relatable conflict</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>She told me I was boring. So I did this.</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Story — challenge accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>I planned a date in 2 minutes and she talked about it for 3 weeks.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Result story</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>My girlfriend literally said 'who are you and what did you do with my boyfriend.'</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Reaction story</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>She posted about our date night before we even got home.</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Social proof / she was impressed</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>I used to be the 'wanna just watch Netflix?' guy. Not anymore.</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Transformation story</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>My girl started bragging about our dates to her friends. Here's why.</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Social validation story</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>She asked me how I keep coming up with date ideas. I'll never tell her.</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Secret weapon story</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>I went from 'you never plan anything' to 'how do you always know what to do.'</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Before/after quote</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>POV: You actually plan a date and she can't stop smiling.</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>POV format</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>POV: She realizes you planned the whole night without her asking.</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>POV format</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Her friends are asking where she found you. Thank this app.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Third-party validation</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>When she says 'surprise me' and you actually can.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Relatable challenge solved</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>The look on her face when she realizes you planned the whole thing.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Emotional payoff</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>3 date ideas that cost less than your DoorDash order.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Budget-friendly value</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>5 date ideas she's never heard of.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Novelty / listicle</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Date ideas that aren't dinner and a movie. You're welcome.</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Anti-basic list</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Here's a date idea that'll cost you $0 and she'll love it.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Free date hook</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>The $15 date that hits harder than a $200 dinner.</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Budget vs expensive comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Date ideas for guys who think they're not creative.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Relatable identity</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Winter date ideas that aren't Netflix on the couch.</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Seasonal + anti-lazy</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Rainy day date ideas that she'll actually love.</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Situational</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>At-home date ideas that don't feel like giving up.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>At-home reframe</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Date ideas for when you're broke but still wanna impress her.</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Budget-conscious</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>She doesn't want expensive. She wants intentional.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Reframe — effort over money</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>The difference between a good boyfriend and a great one is a plan.</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Identity-level</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Women remember how you made them feel. Not where you took them.</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Emotional insight</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>She's not high maintenance. You're just low effort.</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Spicy reframe</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>A planned date says 'I was thinking about you.' That's the whole point.</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Why it matters</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>It's not about the money. It's about the fact that you tried.</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Effort framing</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>The most attractive thing a guy can do is plan without being asked.</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Attraction angle</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>She fell in love with the guy who planned things. Be that guy again.</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Nostalgia / identity</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>You used to plan dates when you were trying to get her. Don't stop now.</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Early relationship comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Effort is the love language nobody talks about.</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Love language reframe</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Her: 'Where are we going?' You: 'It's a surprise.' Her: *melts*</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Text-on-screen skit</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Me googling 'date ideas' for the 47th time this year.</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Relatable meme</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>When she says 'I don't care where we go' but you know she definitely cares.</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Relatable moment</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Her Pinterest board has 200 date ideas. You have zero. Fix that.</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Funny comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>My brain when she asks 'what are we doing this weekend': *dial-up internet sound*</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Meme format</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Netflix and chill stopped being impressive 3 months in.</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Funny truth</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>She saved 47 date ideas on Instagram. You opened none.</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Specific number comedy</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>You planned one creative date and she told everyone she knows.</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Funny truth about women sharing</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>The 'I don't know, what do you wanna do' cycle ends here.</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Breaking the loop</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>When your girl sends you a reel that says 'why don't we ever do this?' Take the hint.</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Relatable hint-dropping</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Unpopular opinion: Most guys aren't bad boyfriends. They're just bad planners.</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Unpopular opinion format</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Hot take: If you can plan a fantasy football draft, you can plan a date.</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Comparison callout</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Controversial but true: She doesn't need more gifts. She needs more plans.</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Gifts vs experiences</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>I'm gonna say what she won't: She's bored. Do something about it.</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Blunt honesty</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Flowers die. Dates become memories. Plan better.</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Poetic hot take</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Your competition isn't other guys. It's her deciding she deserves better.</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Stakes-raising</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>If she stopped asking you to go on dates, she didn't stop wanting to.</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Worrying realization</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>She's not nagging. She's literally telling you what she needs.</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Reframe nagging</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>I found something that's about to change your relationship.</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Curiosity gap</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>There's an app that plans your entire date night. Why is no one talking about this?</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Discovery / why isn't this bigger</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Wait, you guys are still googling date ideas?</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>You guys meme format</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>I can't believe this is free.</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Disbelief hook</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>This app just did in 2 minutes what I couldn't do in 2 hours.</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Time comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Tell me you're a good boyfriend without telling me you're a good boyfriend.</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Trend format</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>One thing I wish I knew earlier about relationships.</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Wisdom hook</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>This is going to sound crazy but hear me out.</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Pattern interrupt</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>I don't usually recommend apps but this one's different.</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Exception framing</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>You're one good date away from being her favorite person again.</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Hopeful + actionable</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Fellas, screenshot this. You'll need it.</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Save / screenshot CTA</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Save this for when she says 'we never do anything.'</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Save for later</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Save this before your girl sees it and sends it to you.</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Funny save CTA</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Show this to your man. He needs it.</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Targeting the girlfriend watching</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Tag your boyfriend. He needs to see this.</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Tag CTA — girlfriend audience</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>If you're watching this with your girl right now, the pressure is on.</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Real-time pressure</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Alright, no more excuses after this one.</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>No excuses closer</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Your move, fellas.</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Short challenge CTA</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>She remembers the dates you planned. Not the ones she had to suggest.</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Memory / effort angle</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Two minutes of planning. A whole night she won't forget.</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Time-to-impact ratio</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E16"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>